<commit_message>
I made that scripts automaticly write the input values of vin and id into the excel worksheets
</commit_message>
<xml_diff>
--- a/Cars.xlsx
+++ b/Cars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dusza\Desktop\Cars\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dusza\Desktop\cars_analysys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E844183D-18AF-4EAB-B803-8DCE897E6C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A61B0A-8C23-4818-866E-0FB974094178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cars" sheetId="1" r:id="rId1"/>
@@ -19,82 +19,101 @@
     <sheet name="Sellers" sheetId="4" r:id="rId4"/>
     <sheet name="Customers" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+  <si>
+    <t>vin</t>
+  </si>
+  <si>
+    <t>car_name</t>
+  </si>
+  <si>
+    <t>car_manufacturer</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>engine</t>
+  </si>
+  <si>
+    <t>transmission_type</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>retail_price</t>
+  </si>
+  <si>
+    <t>current_price</t>
+  </si>
+  <si>
+    <t>seller_id</t>
+  </si>
+  <si>
+    <t>buyer_id</t>
+  </si>
+  <si>
+    <t>25F9N5NXM4IGC4342</t>
+  </si>
+  <si>
+    <t>LHMONS7M2F1OKPRT3</t>
+  </si>
+  <si>
+    <t>DTWGB2ODEO4XOALNU</t>
+  </si>
+  <si>
+    <t>76178I4Z4JVTBKD0R</t>
+  </si>
+  <si>
+    <t>BPEVHNWEWII29IHOX</t>
+  </si>
+  <si>
+    <t>AAV7P62EF2GFVF1XL</t>
+  </si>
+  <si>
+    <t>SQF6J5UHM1E</t>
+  </si>
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>car_name</t>
-  </si>
-  <si>
     <t>manufacturer</t>
   </si>
   <si>
+    <t>funded</t>
+  </si>
+  <si>
+    <t>headquarters</t>
+  </si>
+  <si>
+    <t>number_of_employees</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
-    <t>car_manufacturer</t>
+    <t>fuel_type</t>
   </si>
   <si>
     <t>release_date</t>
   </si>
   <si>
-    <t>engine</t>
-  </si>
-  <si>
-    <t>fuel_type</t>
-  </si>
-  <si>
-    <t>retail_price</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>current_price</t>
-  </si>
-  <si>
-    <t>vin</t>
-  </si>
-  <si>
-    <t>transmission_type</t>
-  </si>
-  <si>
-    <t>used</t>
-  </si>
-  <si>
-    <t>funded</t>
-  </si>
-  <si>
-    <t>headquarters</t>
-  </si>
-  <si>
-    <t>number_of_employees</t>
-  </si>
-  <si>
     <t>surname</t>
   </si>
   <si>
     <t>nationality</t>
   </si>
   <si>
+    <t>DJ41R7T8LTT</t>
+  </si>
+  <si>
     <t>customer_id</t>
-  </si>
-  <si>
-    <t>seller_id</t>
-  </si>
-  <si>
-    <t>buyer_id</t>
   </si>
 </sst>
 </file>
@@ -412,9 +431,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -433,37 +452,72 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -472,7 +526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97DEF82-F543-4283-A499-6FBD4F08B360}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -489,19 +543,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -510,7 +564,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6802D73-19DF-4332-92C8-3E36F574706E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -526,16 +580,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -544,15 +598,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946C2CDB-5043-4F72-8380-463487E18655}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
@@ -560,16 +615,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -578,7 +638,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20E331B-5033-468E-BE2C-490247136017}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -595,16 +655,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created a script that fills the cells with random name and surname NOTE: script inputs values into wrong rows as for now
</commit_message>
<xml_diff>
--- a/Cars.xlsx
+++ b/Cars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dusza\Desktop\cars_analysys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A61B0A-8C23-4818-866E-0FB974094178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D9AB5B-024B-4909-B419-83B686895CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cars" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
   <si>
     <t>vin</t>
   </si>
@@ -59,27 +59,6 @@
     <t>buyer_id</t>
   </si>
   <si>
-    <t>25F9N5NXM4IGC4342</t>
-  </si>
-  <si>
-    <t>LHMONS7M2F1OKPRT3</t>
-  </si>
-  <si>
-    <t>DTWGB2ODEO4XOALNU</t>
-  </si>
-  <si>
-    <t>76178I4Z4JVTBKD0R</t>
-  </si>
-  <si>
-    <t>BPEVHNWEWII29IHOX</t>
-  </si>
-  <si>
-    <t>AAV7P62EF2GFVF1XL</t>
-  </si>
-  <si>
-    <t>SQF6J5UHM1E</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -110,10 +89,157 @@
     <t>nationality</t>
   </si>
   <si>
-    <t>DJ41R7T8LTT</t>
+    <t>P32ENXGVCCS</t>
+  </si>
+  <si>
+    <t>TZ3T7UARQ7G</t>
+  </si>
+  <si>
+    <t>AV4E00KSHI9</t>
+  </si>
+  <si>
+    <t>LCTFGCLX1S1</t>
+  </si>
+  <si>
+    <t>0HICEO4ZY9E</t>
+  </si>
+  <si>
+    <t>EIOW0MABK3N</t>
+  </si>
+  <si>
+    <t>QQ5BYS6K7TT</t>
+  </si>
+  <si>
+    <t>CPGOZCP26RF</t>
+  </si>
+  <si>
+    <t>QX1PRL5CYSY</t>
+  </si>
+  <si>
+    <t>60DC3OO6WOR</t>
+  </si>
+  <si>
+    <t>A9M6AGS10SP</t>
+  </si>
+  <si>
+    <t>3WR4UL2I5HZ</t>
+  </si>
+  <si>
+    <t>OL4N8TGNWU9</t>
+  </si>
+  <si>
+    <t>FPHLBJSUDW9</t>
+  </si>
+  <si>
+    <t>GGY0TGA6D3X</t>
+  </si>
+  <si>
+    <t>G6YL6I1FSL0</t>
+  </si>
+  <si>
+    <t>ENL4P17OHCK</t>
+  </si>
+  <si>
+    <t>04690GATVX2</t>
+  </si>
+  <si>
+    <t>1HN15CUA28G</t>
+  </si>
+  <si>
+    <t>NQI2IY62MDM</t>
+  </si>
+  <si>
+    <t>V0BE4PGNOD3</t>
+  </si>
+  <si>
+    <t>QKM90ML5A30</t>
+  </si>
+  <si>
+    <t>48OCBSIHTXM</t>
+  </si>
+  <si>
+    <t>69DJSG7L52K</t>
+  </si>
+  <si>
+    <t>1UT6MA4WJ2Z</t>
+  </si>
+  <si>
+    <t>K3SC99B2BZR</t>
+  </si>
+  <si>
+    <t>WLNN5I8IQ9K</t>
+  </si>
+  <si>
+    <t>Z78IAAHX6Y8</t>
+  </si>
+  <si>
+    <t>47544KSZTVT</t>
+  </si>
+  <si>
+    <t>34AYLM8E9N2</t>
+  </si>
+  <si>
+    <t>4IDNEHMNJEZ</t>
+  </si>
+  <si>
+    <t>YF8AFVR8RY1</t>
+  </si>
+  <si>
+    <t>OWE962XBNMV</t>
+  </si>
+  <si>
+    <t>Y8FHL5HGT45</t>
+  </si>
+  <si>
+    <t>P1DKDE5YD02</t>
+  </si>
+  <si>
+    <t>TGCBUWQIBEH</t>
+  </si>
+  <si>
+    <t>SAHLAAJYCO9</t>
+  </si>
+  <si>
+    <t>ZVW7HBEL3QJ</t>
+  </si>
+  <si>
+    <t>RE5FG8D9QAB</t>
+  </si>
+  <si>
+    <t>L3PTC6MEYOO</t>
+  </si>
+  <si>
+    <t>L9ZBKWE5JVC</t>
+  </si>
+  <si>
+    <t>ZD01CFWUWHW</t>
+  </si>
+  <si>
+    <t>E72ANOG1P4X</t>
+  </si>
+  <si>
+    <t>QPZWVQNG06Y</t>
+  </si>
+  <si>
+    <t>5KJE1GLFWJF</t>
+  </si>
+  <si>
+    <t>C6LFXUFO3QX</t>
+  </si>
+  <si>
+    <t>0J0RTVGLCVJ</t>
+  </si>
+  <si>
+    <t>IL82K5E5HXC</t>
+  </si>
+  <si>
+    <t>C61T6YM7RB1</t>
   </si>
   <si>
     <t>customer_id</t>
+  </si>
+  <si>
+    <t>KYEICXVQQNM</t>
   </si>
 </sst>
 </file>
@@ -431,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,41 +611,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -529,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -543,19 +634,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -568,7 +659,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,16 +671,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -599,10 +690,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,18 +709,258 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -639,7 +970,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
@@ -655,16 +986,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>